<commit_message>
Changes to remove unnecessary files.
</commit_message>
<xml_diff>
--- a/evograph/analysis/degreeDistribution.xlsx
+++ b/evograph/analysis/degreeDistribution.xlsx
@@ -9,13 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17600" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$B$1:$N$22</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$B$2:$M$24</definedName>
   </definedNames>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="52">
   <si>
     <t>In Degree Distribution</t>
   </si>
@@ -179,13 +179,13 @@
     <t>Vertices</t>
   </si>
   <si>
-    <t>Expected Upscale</t>
-  </si>
-  <si>
     <t>k=3</t>
   </si>
   <si>
     <t>k=4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Degree Distribution </t>
   </si>
 </sst>
 </file>
@@ -221,18 +221,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -242,7 +236,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="1" tint="0.499984740745262"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -309,13 +303,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -329,26 +317,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -363,6 +332,29 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -645,10 +637,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:N27"/>
+  <dimension ref="B2:M35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="B2" sqref="B2:G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -656,600 +648,645 @@
     <col min="1" max="1" width="10.83203125" customWidth="1"/>
     <col min="3" max="3" width="19.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.83203125" customWidth="1"/>
-    <col min="8" max="8" width="1.1640625" style="14" customWidth="1"/>
-    <col min="10" max="10" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.33203125" customWidth="1"/>
+    <col min="8" max="8" width="11.1640625" customWidth="1"/>
+    <col min="9" max="9" width="14.83203125" customWidth="1"/>
+    <col min="12" max="12" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11" customWidth="1"/>
+    <col min="17" max="17" width="11.33203125" customWidth="1"/>
+    <col min="18" max="19" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="D1" s="17" t="s">
-        <v>49</v>
-      </c>
-      <c r="E1" s="17"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="19"/>
-      <c r="L1" s="19"/>
-      <c r="M1" s="12"/>
-      <c r="N1" s="12"/>
-    </row>
-    <row r="2" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="20"/>
+    <row r="2" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="D2" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="E2" s="21"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
       <c r="J2" s="20"/>
       <c r="K2" s="20"/>
-      <c r="L2" s="20"/>
-      <c r="M2" s="20"/>
-      <c r="N2" s="20"/>
-    </row>
-    <row r="3" spans="2:14" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="9" t="s">
+      <c r="L2" s="10"/>
+      <c r="M2" s="10"/>
+    </row>
+    <row r="3" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="17"/>
+      <c r="K3" s="17"/>
+      <c r="L3" s="10"/>
+      <c r="M3" s="10"/>
+    </row>
+    <row r="4" spans="2:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="22"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" s="22"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="19"/>
+      <c r="J4" s="19"/>
+      <c r="K4" s="19"/>
+      <c r="L4" s="19"/>
+      <c r="M4" s="19"/>
+    </row>
+    <row r="5" spans="2:13" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C5" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D5" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E5" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F5" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="G5" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="H3" s="13"/>
-      <c r="I3" s="21"/>
-      <c r="J3" s="21"/>
-      <c r="K3" s="21"/>
-      <c r="L3" s="21"/>
-      <c r="M3" s="21"/>
-      <c r="N3" s="21"/>
-    </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H4" s="13"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="12"/>
-      <c r="K4" s="22"/>
-      <c r="L4" s="12"/>
-      <c r="M4" s="12"/>
-      <c r="N4" s="22"/>
-    </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H5" s="13"/>
+      <c r="H5" s="12"/>
       <c r="I5" s="12"/>
       <c r="J5" s="12"/>
-      <c r="K5" s="22"/>
+      <c r="K5" s="12"/>
       <c r="L5" s="12"/>
       <c r="M5" s="12"/>
-      <c r="N5" s="22"/>
-    </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="10"/>
+      <c r="L6" s="10"/>
+      <c r="M6" s="13"/>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="13"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="10"/>
+      <c r="M7" s="13"/>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
         <v>3</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C8" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="E8" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F8" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="G8" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="H6" s="13"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="22"/>
-      <c r="L6" s="12"/>
-      <c r="M6" s="12"/>
-      <c r="N6" s="22"/>
-    </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="C7" s="2" t="s">
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="13"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="10"/>
+      <c r="M8" s="13"/>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="C9" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D9" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E7" s="8"/>
-      <c r="F7" s="4" t="s">
+      <c r="E9" s="6"/>
+      <c r="F9" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="G9" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="H7" s="13"/>
-      <c r="I7" s="12"/>
-      <c r="J7" s="23"/>
-      <c r="K7" s="24"/>
-      <c r="L7" s="12"/>
-      <c r="M7" s="23"/>
-      <c r="N7" s="24"/>
-    </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="C8" s="2"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="13"/>
-      <c r="I8" s="12"/>
-      <c r="J8" s="23"/>
-      <c r="K8" s="22"/>
-      <c r="L8" s="12"/>
-      <c r="M8" s="23"/>
-      <c r="N8" s="22"/>
-    </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B9" s="9" t="s">
+      <c r="H9" s="10"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="14"/>
+      <c r="M9" s="15"/>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="C10" s="2"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="13"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="14"/>
+      <c r="M10" s="13"/>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B11" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C11" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="D11" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E9" s="11" t="s">
+      <c r="E11" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="F9" s="10" t="s">
+      <c r="F11" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="G9" s="9" t="s">
+      <c r="G11" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="H9" s="13"/>
-      <c r="I9" s="21"/>
-      <c r="J9" s="21"/>
-      <c r="K9" s="21"/>
-      <c r="L9" s="21"/>
-      <c r="M9" s="21"/>
-      <c r="N9" s="21"/>
-    </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B10" t="s">
-        <v>1</v>
-      </c>
-      <c r="C10" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H10" s="13"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="12"/>
-      <c r="K10" s="22"/>
-      <c r="L10" s="12"/>
-      <c r="M10" s="12"/>
-      <c r="N10" s="22"/>
-    </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B11" t="s">
-        <v>2</v>
-      </c>
-      <c r="C11" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E11" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H11" s="13"/>
+      <c r="H11" s="12"/>
       <c r="I11" s="12"/>
       <c r="J11" s="12"/>
-      <c r="K11" s="22"/>
+      <c r="K11" s="12"/>
       <c r="L11" s="12"/>
       <c r="M11" s="12"/>
-      <c r="N11" s="22"/>
-    </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="13"/>
+      <c r="K12" s="10"/>
+      <c r="L12" s="10"/>
+      <c r="M12" s="13"/>
+    </row>
+    <row r="13" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="13"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="10"/>
+      <c r="M13" s="13"/>
+    </row>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
         <v>3</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C14" t="s">
         <v>13</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D14" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E12" s="8" t="s">
+      <c r="E14" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="F14" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="G14" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="H12" s="13"/>
-      <c r="I12" s="12"/>
-      <c r="J12" s="12"/>
-      <c r="K12" s="22"/>
-      <c r="L12" s="12"/>
-      <c r="M12" s="12"/>
-      <c r="N12" s="22"/>
-    </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B13" t="s">
+      <c r="H14" s="10"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="13"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="10"/>
+      <c r="M14" s="13"/>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
         <v>4</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C15" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D15" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="E15" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="F15" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="G13" s="1" t="s">
+      <c r="G15" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H13" s="13"/>
-      <c r="I13" s="12"/>
-      <c r="J13" s="12"/>
-      <c r="K13" s="22"/>
-      <c r="L13" s="12"/>
-      <c r="M13" s="12"/>
-      <c r="N13" s="22"/>
-    </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="C14" s="2" t="s">
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="13"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="10"/>
+      <c r="M15" s="13"/>
+    </row>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="C16" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D16" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="E14" s="8"/>
-      <c r="F14" s="4" t="s">
+      <c r="E16" s="6"/>
+      <c r="F16" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="G14" s="5" t="s">
+      <c r="G16" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="H14" s="13"/>
-      <c r="I14" s="12"/>
-      <c r="J14" s="23"/>
-      <c r="K14" s="24"/>
-      <c r="L14" s="12"/>
-      <c r="M14" s="23"/>
-      <c r="N14" s="24"/>
-    </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="C15" s="2"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="13"/>
-      <c r="I15" s="12"/>
-      <c r="J15" s="23"/>
-      <c r="K15" s="22"/>
-      <c r="L15" s="12"/>
-      <c r="M15" s="23"/>
-      <c r="N15" s="22"/>
-    </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B16" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="C16" s="9" t="s">
+      <c r="H16" s="10"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="15"/>
+      <c r="K16" s="10"/>
+      <c r="L16" s="14"/>
+      <c r="M16" s="15"/>
+    </row>
+    <row r="17" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="C17" s="2"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="10"/>
+      <c r="I17" s="14"/>
+      <c r="J17" s="13"/>
+      <c r="K17" s="10"/>
+      <c r="L17" s="14"/>
+      <c r="M17" s="13"/>
+    </row>
+    <row r="18" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B18" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C18" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="D16" s="9" t="s">
+      <c r="D18" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E16" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="F16" s="10" t="s">
+      <c r="E18" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="F18" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="G16" s="9" t="s">
+      <c r="G18" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="H16" s="13"/>
-      <c r="I16" s="21"/>
-      <c r="J16" s="21"/>
-      <c r="K16" s="21"/>
-      <c r="L16" s="21"/>
-      <c r="M16" s="21"/>
-      <c r="N16" s="21"/>
-    </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B17" t="s">
-        <v>1</v>
-      </c>
-      <c r="C17" t="s">
-        <v>14</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E17" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="H17" s="13"/>
-      <c r="I17" s="12"/>
-      <c r="J17" s="12"/>
-      <c r="K17" s="22"/>
-      <c r="L17" s="12"/>
-      <c r="M17" s="12"/>
-      <c r="N17" s="22"/>
-    </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B18" t="s">
-        <v>2</v>
-      </c>
-      <c r="C18" t="s">
-        <v>15</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E18" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H18" s="13"/>
+      <c r="H18" s="12"/>
       <c r="I18" s="12"/>
       <c r="J18" s="12"/>
-      <c r="K18" s="22"/>
+      <c r="K18" s="12"/>
       <c r="L18" s="12"/>
       <c r="M18" s="12"/>
-      <c r="N18" s="22"/>
-    </row>
-    <row r="19" spans="2:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19" t="s">
+        <v>14</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H19" s="10"/>
+      <c r="I19" s="10"/>
+      <c r="J19" s="13"/>
+      <c r="K19" s="10"/>
+      <c r="L19" s="10"/>
+      <c r="M19" s="13"/>
+    </row>
+    <row r="20" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>2</v>
+      </c>
+      <c r="C20" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H20" s="10"/>
+      <c r="I20" s="10"/>
+      <c r="J20" s="13"/>
+      <c r="K20" s="10"/>
+      <c r="L20" s="10"/>
+      <c r="M20" s="13"/>
+    </row>
+    <row r="21" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
         <v>3</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C21" t="s">
         <v>16</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D21" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E19" s="8" t="s">
+      <c r="E21" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="F19" s="3" t="s">
+      <c r="F21" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="G19" s="1" t="s">
+      <c r="G21" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="H19" s="13"/>
-      <c r="I19" s="12"/>
-      <c r="J19" s="12"/>
-      <c r="K19" s="22"/>
-      <c r="L19" s="12"/>
-      <c r="M19" s="12"/>
-      <c r="N19" s="22"/>
-    </row>
-    <row r="20" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B20" t="s">
+      <c r="H21" s="10"/>
+      <c r="I21" s="10"/>
+      <c r="J21" s="13"/>
+      <c r="K21" s="10"/>
+      <c r="L21" s="10"/>
+      <c r="M21" s="13"/>
+    </row>
+    <row r="22" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
         <v>4</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="D22" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E20" s="8" t="s">
+      <c r="E22" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="F20" s="3" t="s">
+      <c r="F22" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="G20" s="1" t="s">
+      <c r="G22" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H20" s="13"/>
-      <c r="I20" s="12"/>
-      <c r="J20" s="12"/>
-      <c r="K20" s="22"/>
-      <c r="L20" s="12"/>
-      <c r="M20" s="12"/>
-      <c r="N20" s="22"/>
-    </row>
-    <row r="21" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B21" t="s">
+      <c r="H22" s="10"/>
+      <c r="I22" s="10"/>
+      <c r="J22" s="13"/>
+      <c r="K22" s="10"/>
+      <c r="L22" s="10"/>
+      <c r="M22" s="13"/>
+    </row>
+    <row r="23" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B23" t="s">
         <v>7</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C23" t="s">
         <v>10</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="D23" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E21" s="8" t="s">
+      <c r="E23" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F21" s="3"/>
-      <c r="G21" s="1" t="s">
+      <c r="F23" s="3"/>
+      <c r="G23" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="H21" s="13"/>
-      <c r="I21" s="12"/>
-      <c r="J21" s="12"/>
-      <c r="K21" s="22"/>
-      <c r="L21" s="12"/>
-      <c r="M21" s="12"/>
-      <c r="N21" s="22"/>
-    </row>
-    <row r="22" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="C22" s="2" t="s">
+      <c r="H23" s="10"/>
+      <c r="I23" s="10"/>
+      <c r="J23" s="13"/>
+      <c r="K23" s="10"/>
+      <c r="L23" s="10"/>
+      <c r="M23" s="13"/>
+    </row>
+    <row r="24" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="C24" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D22" s="6">
+      <c r="D24" s="25">
         <v>3.17</v>
       </c>
-      <c r="E22" s="8"/>
-      <c r="F22" s="4" t="s">
+      <c r="E24" s="6"/>
+      <c r="F24" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="G22" s="7">
+      <c r="G24" s="26">
         <v>2.25</v>
       </c>
-      <c r="H22" s="13"/>
-      <c r="I22" s="12"/>
-      <c r="J22" s="23"/>
-      <c r="K22" s="25"/>
-      <c r="L22" s="12"/>
-      <c r="M22" s="23"/>
-      <c r="N22" s="26"/>
-    </row>
-    <row r="23" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="H23" s="13"/>
-      <c r="I23" s="12"/>
-      <c r="J23" s="12"/>
-      <c r="K23" s="12"/>
-      <c r="L23" s="12"/>
-      <c r="M23" s="12"/>
-      <c r="N23" s="12"/>
-    </row>
-    <row r="24" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B24" t="s">
-        <v>51</v>
-      </c>
-      <c r="I24" s="12"/>
-      <c r="J24" s="12"/>
-      <c r="K24" s="12"/>
-      <c r="L24" s="12"/>
-      <c r="M24" s="12"/>
-      <c r="N24" s="12"/>
-    </row>
-    <row r="25" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="I25" s="12"/>
-      <c r="J25" s="12"/>
-      <c r="K25" s="12"/>
-      <c r="L25" s="12"/>
-      <c r="M25" s="12"/>
-      <c r="N25" s="12"/>
-    </row>
-    <row r="26" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="I26" s="14"/>
-      <c r="J26" s="14"/>
-      <c r="K26" s="14"/>
-      <c r="L26" s="14"/>
-      <c r="M26" s="14"/>
-      <c r="N26" s="14"/>
-    </row>
-    <row r="27" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="I27" s="14"/>
-      <c r="J27" s="14"/>
-      <c r="K27" s="14"/>
-      <c r="L27" s="14"/>
-      <c r="M27" s="14"/>
-      <c r="N27" s="14"/>
+      <c r="H24" s="10"/>
+      <c r="I24" s="14"/>
+      <c r="J24" s="16"/>
+      <c r="K24" s="10"/>
+      <c r="L24" s="14"/>
+      <c r="M24" s="17"/>
+    </row>
+    <row r="25" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="E25" s="6"/>
+      <c r="H25" s="10"/>
+      <c r="I25" s="10"/>
+      <c r="J25" s="10"/>
+      <c r="K25" s="10"/>
+      <c r="L25" s="10"/>
+      <c r="M25" s="10"/>
+    </row>
+    <row r="26" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B26" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D26" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="E26" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="F26" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="G26" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="H26" s="10"/>
+      <c r="I26" s="10"/>
+      <c r="J26" s="10"/>
+      <c r="K26" s="10"/>
+      <c r="L26" s="10"/>
+      <c r="M26" s="10"/>
+    </row>
+    <row r="27" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B27" t="s">
+        <v>1</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="H27" s="10"/>
+      <c r="I27" s="10"/>
+      <c r="J27" s="10"/>
+      <c r="K27" s="10"/>
+      <c r="L27" s="10"/>
+      <c r="M27" s="10"/>
+    </row>
+    <row r="28" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B28" t="s">
+        <v>2</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="H28" s="11"/>
+      <c r="I28" s="11"/>
+      <c r="J28" s="11"/>
+      <c r="K28" s="11"/>
+      <c r="L28" s="11"/>
+      <c r="M28" s="11"/>
+    </row>
+    <row r="29" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B29" t="s">
+        <v>3</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="H29" s="11"/>
+      <c r="I29" s="11"/>
+      <c r="J29" s="11"/>
+      <c r="K29" s="11"/>
+      <c r="L29" s="11"/>
+      <c r="M29" s="11"/>
+    </row>
+    <row r="30" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
+        <v>4</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="31" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B31" t="s">
+        <v>7</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="35" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C35" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>21</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="L2:N2"/>
-    <mergeCell ref="K1:L1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="I2:K2"/>
+  <mergeCells count="3">
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="E4:G4"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="69" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup scale="71" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
   <colBreaks count="1" manualBreakCount="1">
-    <brk id="16" max="1048575" man="1"/>
+    <brk id="15" max="1048575" man="1"/>
   </colBreaks>
   <ignoredErrors>
-    <ignoredError sqref="D20 G21" twoDigitTextYear="1"/>
-    <ignoredError sqref="D14 D7 G7 G14" numberStoredAsText="1"/>
+    <ignoredError sqref="D22 G23" twoDigitTextYear="1"/>
+    <ignoredError sqref="D16 D9 G9 G16" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Information added to readme
</commit_message>
<xml_diff>
--- a/evograph/analysis/degreeDistribution.xlsx
+++ b/evograph/analysis/degreeDistribution.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="51">
   <si>
     <t>In Degree Distribution</t>
   </si>
@@ -180,9 +180,6 @@
   </si>
   <si>
     <t>k=3</t>
-  </si>
-  <si>
-    <t>k=4</t>
   </si>
   <si>
     <t xml:space="preserve">Degree Distribution </t>
@@ -293,7 +290,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -339,6 +336,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -351,10 +354,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -640,7 +640,7 @@
   <dimension ref="B2:M35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:G24"/>
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -658,10 +658,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="D2" s="21" t="s">
-        <v>51</v>
-      </c>
-      <c r="E2" s="21"/>
+      <c r="D2" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2" s="23"/>
       <c r="H2" s="10"/>
       <c r="I2" s="10"/>
       <c r="J2" s="20"/>
@@ -680,16 +680,16 @@
       <c r="M3" s="10"/>
     </row>
     <row r="4" spans="2:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="22"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="24" t="s">
+      <c r="C4" s="24"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="F4" s="22"/>
-      <c r="G4" s="22"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
       <c r="H4" s="19"/>
       <c r="I4" s="19"/>
       <c r="J4" s="19"/>
@@ -1154,14 +1154,14 @@
       <c r="C24" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D24" s="25">
+      <c r="D24" s="21">
         <v>3.17</v>
       </c>
       <c r="E24" s="6"/>
       <c r="F24" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="G24" s="26">
+      <c r="G24" s="22">
         <v>2.25</v>
       </c>
       <c r="H24" s="10"/>
@@ -1181,24 +1181,12 @@
       <c r="M25" s="10"/>
     </row>
     <row r="26" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B26" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="C26" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="D26" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="E26" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="F26" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="G26" s="18" t="s">
-        <v>20</v>
-      </c>
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="27"/>
+      <c r="E26" s="8"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="18"/>
       <c r="H26" s="10"/>
       <c r="I26" s="10"/>
       <c r="J26" s="10"/>
@@ -1207,12 +1195,8 @@
       <c r="M26" s="10"/>
     </row>
     <row r="27" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B27" t="s">
-        <v>1</v>
-      </c>
-      <c r="E27" s="6" t="s">
-        <v>43</v>
-      </c>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
       <c r="H27" s="10"/>
       <c r="I27" s="10"/>
       <c r="J27" s="10"/>
@@ -1221,12 +1205,8 @@
       <c r="M27" s="10"/>
     </row>
     <row r="28" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B28" t="s">
-        <v>2</v>
-      </c>
-      <c r="E28" s="6" t="s">
-        <v>44</v>
-      </c>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
       <c r="H28" s="11"/>
       <c r="I28" s="11"/>
       <c r="J28" s="11"/>
@@ -1235,12 +1215,8 @@
       <c r="M28" s="11"/>
     </row>
     <row r="29" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B29" t="s">
-        <v>3</v>
-      </c>
-      <c r="E29" s="6" t="s">
-        <v>45</v>
-      </c>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
       <c r="H29" s="11"/>
       <c r="I29" s="11"/>
       <c r="J29" s="11"/>
@@ -1249,28 +1225,16 @@
       <c r="M29" s="11"/>
     </row>
     <row r="30" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B30" t="s">
-        <v>4</v>
-      </c>
-      <c r="E30" s="6" t="s">
-        <v>46</v>
-      </c>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
     </row>
     <row r="31" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B31" t="s">
-        <v>7</v>
-      </c>
-      <c r="E31" s="6" t="s">
-        <v>47</v>
-      </c>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
     </row>
     <row r="35" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C35" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F35" s="2" t="s">
-        <v>21</v>
-      </c>
+      <c r="C35" s="2"/>
+      <c r="F35" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>